<commit_message>
MAS-452 try using a map instead of a list for comparisons
</commit_message>
<xml_diff>
--- a/src/test/resources/compare-tiers/test/delius/wmt_ps.xlsx
+++ b/src/test/resources/compare-tiers/test/delius/wmt_ps.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark.rees/workspace/hmpps-tier/src/test/resources/compare-tiers/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark.rees/workspace/hmpps-tier/src/test/resources/compare-tiers/test/delius/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57BF3FA-4EFF-B842-83F5-CF7F88761F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C29E88F-7D46-FC43-B7D1-387A8F311983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="349">
   <si>
     <t>Trust</t>
   </si>
@@ -1139,6 +1139,9 @@
   </si>
   <si>
     <t>X123415</t>
+  </si>
+  <si>
+    <t>X123499</t>
   </si>
 </sst>
 </file>
@@ -6174,7 +6177,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6578,13 +6581,27 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
+      <c r="A18" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>124</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>